<commit_message>
new base design, rewrite start, defense code
</commit_message>
<xml_diff>
--- a/basedesign.xlsx
+++ b/basedesign.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lubos/Documents/Projects/screeps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4F15AA0-32F7-3546-94CD-E4539951DB68}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99E8DE71-30F2-2747-BF68-A48D8828B9F3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4040" yWindow="3080" windowWidth="27440" windowHeight="16560" xr2:uid="{1D64CEC5-90FC-5447-9D59-01EDF2F78035}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="22">
   <si>
     <t>Screeps Base Design</t>
   </si>
@@ -61,6 +61,36 @@
   </si>
   <si>
     <t>https://screeps.arcath.net/building-planner/?share=N4IgdghgtgpiBcIQBoQGcAWEBOATB6WeADCiNgMYA2CAHKgEYCuAllbi2AOZoKhoAXAPbYIXOPFAAHIb3gBtUAA8EAJgDMqAJ5riAXwC6e1NiER8kkDLmKQK+KtXaEARgCcx5Ws0gd8d552agAszv4eyF4Oob66gfaOYar6kUEOTrEOLvEhSdmpCT5+qvlRJWEBBWoZfi60OVkVAOwNyRX1VdHtrQCsFRFlAGzdnap9mS4tozXVrS55rcRJqnNJ6otrrcOZGlvLvZujMcUro+PFpWmqx66DrU39rfQ7KWUPO5f27guddUmvaW+EwGgPeFwaLm2Jwh528EKhIQhYLUPQhz2KqN+6LUd1+biSwQh+J2UzKSx2HTK8x2IISM3g6gBhTCjNaNwZTJRSVpOKSlKuyIcpKu2IcuLKxIxDUZBOl1OK606Mp2pwlPzK9OurSKKLZSXFV1hQtamoNCXlamFCUFWtGorGep2hOm3MdxR5Dh1-kxGoqdyMqAEMGwUE4EBolmsCFs5u6AZAVE4AGs+FZZNGyka6oZjCAYEog2A0CwhGBU1GFJn-ntgTXipyxeqBdXRuTah62i9Vl3W02vpK4na+2oB+lpW24aMbYqyvbnW99kOVU9DmqdjOrqPbUNZVOkj7DbuyuyHWd9XXLfdz6MEWKLw4DwkjaeokDoXjV1cLdETfvu8UzV0JIrVcLdH1A68yUgr8-17HZwP8e1PlcG1VUBW9dixI9QU-L57Q3PDF1fG15yuCcf1+Z9SK+DCEMmaDCJJIk+TlbD7GVKVRi3QCHHtEChRY+M0CkCAAHcy0jdNKxg5cz1ksovUcHNAyEUTg3LKSY2qXDcnXbU2O8HSugmfjEhM5SEwgBgNJsBSWNGRTTM1Jz7OPYC3TUflmR2HixlcmTii8wyaQsoQGDQYMADd1Mk2yri9SYLJkNTsAAZRE8SbIzeK-QssAmCTGLpE0uyJnqeNRCgETsAELKFCMPQ9CAA</t>
+  </si>
+  <si>
+    <t>Tw</t>
+  </si>
+  <si>
+    <t>Te</t>
+  </si>
+  <si>
+    <t>Li</t>
+  </si>
+  <si>
+    <t>Má</t>
+  </si>
+  <si>
+    <t>Je</t>
+  </si>
+  <si>
+    <t>Obs</t>
+  </si>
+  <si>
+    <t>pS</t>
+  </si>
+  <si>
+    <t>Nu</t>
+  </si>
+  <si>
+    <t>Tall</t>
+  </si>
+  <si>
+    <t>Wide</t>
   </si>
 </sst>
 </file>
@@ -446,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{794B8A53-C7D6-264E-8846-1732FF91EF00}">
-  <dimension ref="A1:BQ34"/>
+  <dimension ref="A1:BQ43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U3" workbookViewId="0">
-      <selection activeCell="AU20" sqref="AU20"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="AF27" sqref="AF27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -458,7 +488,9 @@
     <col min="25" max="25" width="3.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="2.83203125" style="2"/>
     <col min="27" max="27" width="3.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="28" max="16384" width="2.83203125" style="2"/>
+    <col min="28" max="33" width="2.83203125" style="2"/>
+    <col min="34" max="36" width="3.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="37" max="16384" width="2.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:45" x14ac:dyDescent="0.2">
@@ -2091,7 +2123,9 @@
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
       <c r="Q26" s="1"/>
-      <c r="R26" s="1"/>
+      <c r="R26" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="S26" s="1"/>
       <c r="T26" s="1"/>
       <c r="U26" s="1"/>
@@ -2166,21 +2200,51 @@
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
       <c r="Q27" s="1"/>
-      <c r="R27" s="1"/>
+      <c r="R27" s="1">
+        <v>4</v>
+      </c>
       <c r="S27" s="1"/>
-      <c r="T27" s="1"/>
-      <c r="U27" s="1"/>
-      <c r="V27" s="1"/>
-      <c r="W27" s="1"/>
-      <c r="X27" s="1"/>
-      <c r="Y27" s="1"/>
-      <c r="Z27" s="1"/>
-      <c r="AA27" s="1"/>
-      <c r="AB27" s="1"/>
-      <c r="AC27" s="1"/>
-      <c r="AD27" s="1"/>
+      <c r="T27" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="U27" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="V27" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="W27" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="X27" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y27" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z27" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA27" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB27" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC27" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD27" s="4" t="s">
+        <v>2</v>
+      </c>
       <c r="AE27" s="1"/>
       <c r="AF27" s="1"/>
+      <c r="AI27" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AJ27" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="AZ27" s="1"/>
       <c r="BA27" s="1"/>
       <c r="BB27" s="1" t="s">
@@ -2225,6 +2289,51 @@
       <c r="BO27" s="1"/>
     </row>
     <row r="28" spans="6:69" x14ac:dyDescent="0.2">
+      <c r="R28" s="2">
+        <v>4</v>
+      </c>
+      <c r="T28" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="U28" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="V28" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="W28" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="X28" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y28" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z28" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA28" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AB28" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC28" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD28" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH28" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AI28" s="2">
+        <v>10</v>
+      </c>
+      <c r="AJ28" s="2">
+        <v>10</v>
+      </c>
       <c r="AZ28" s="1"/>
       <c r="BA28" s="1"/>
       <c r="BB28" s="1"/>
@@ -2265,6 +2374,52 @@
       <c r="BO28" s="1"/>
     </row>
     <row r="29" spans="6:69" x14ac:dyDescent="0.2">
+      <c r="R29" s="2">
+        <v>4</v>
+      </c>
+      <c r="T29" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="U29" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="V29" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="W29" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="X29" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y29" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z29" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA29" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB29" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC29" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD29" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH29" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI29" s="2">
+        <v>60</v>
+      </c>
+      <c r="AJ29" s="2">
+        <f>SUM(R27:R39)</f>
+        <v>60</v>
+      </c>
       <c r="AZ29" s="1"/>
       <c r="BA29" s="1"/>
       <c r="BB29" s="1"/>
@@ -2301,6 +2456,51 @@
       <c r="BO29" s="1"/>
     </row>
     <row r="30" spans="6:69" x14ac:dyDescent="0.2">
+      <c r="R30" s="2">
+        <v>6</v>
+      </c>
+      <c r="T30" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="U30" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="V30" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="W30" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="X30" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y30" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z30" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA30" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB30" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC30" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD30" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH30" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI30" s="2">
+        <v>6</v>
+      </c>
+      <c r="AJ30" s="2">
+        <v>6</v>
+      </c>
       <c r="AZ30" s="1"/>
       <c r="BA30" s="1"/>
       <c r="BB30" s="1"/>
@@ -2333,6 +2533,42 @@
       <c r="BO30" s="1"/>
     </row>
     <row r="31" spans="6:69" x14ac:dyDescent="0.2">
+      <c r="R31" s="2">
+        <v>6</v>
+      </c>
+      <c r="T31" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="U31" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="V31" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="W31" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="X31" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y31" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z31" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA31" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB31" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC31" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD31" s="4" t="s">
+        <v>2</v>
+      </c>
       <c r="AZ31" s="1"/>
       <c r="BA31" s="1"/>
       <c r="BB31" s="1"/>
@@ -2362,6 +2598,42 @@
       <c r="BP31" s="1"/>
     </row>
     <row r="32" spans="6:69" x14ac:dyDescent="0.2">
+      <c r="R32" s="2">
+        <v>4</v>
+      </c>
+      <c r="T32" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="U32" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="V32" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="W32" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="X32" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y32" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z32" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA32" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB32" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC32" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD32" s="3" t="s">
+        <v>1</v>
+      </c>
       <c r="AG32" s="1"/>
       <c r="AH32" s="1"/>
       <c r="AI32" s="1"/>
@@ -2386,7 +2658,43 @@
       <c r="BO32" s="1"/>
       <c r="BQ32" s="1"/>
     </row>
-    <row r="33" spans="33:69" x14ac:dyDescent="0.2">
+    <row r="33" spans="18:69" x14ac:dyDescent="0.2">
+      <c r="R33" s="2">
+        <v>2</v>
+      </c>
+      <c r="T33" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="U33" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="V33" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="W33" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="X33" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y33" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z33" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA33" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB33" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC33" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD33" s="4" t="s">
+        <v>2</v>
+      </c>
       <c r="AG33" s="1"/>
       <c r="AH33" s="1"/>
       <c r="AI33" s="1"/>
@@ -2407,12 +2715,248 @@
       <c r="BP33" s="1"/>
       <c r="BQ33" s="1"/>
     </row>
-    <row r="34" spans="33:69" x14ac:dyDescent="0.2">
+    <row r="34" spans="18:69" x14ac:dyDescent="0.2">
+      <c r="R34" s="2">
+        <v>4</v>
+      </c>
+      <c r="T34" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="U34" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="V34" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="W34" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="X34" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y34" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z34" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA34" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB34" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC34" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD34" s="3" t="s">
+        <v>1</v>
+      </c>
       <c r="AY34" s="2" t="s">
         <v>11</v>
       </c>
       <c r="BO34" s="1"/>
       <c r="BP34" s="1"/>
+    </row>
+    <row r="35" spans="18:69" x14ac:dyDescent="0.2">
+      <c r="R35" s="2">
+        <v>2</v>
+      </c>
+      <c r="T35" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="U35" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="V35" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="W35" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="X35" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y35" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z35" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA35" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB35" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC35" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD35" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="18:69" x14ac:dyDescent="0.2">
+      <c r="R36" s="2">
+        <v>4</v>
+      </c>
+      <c r="T36" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="U36" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="V36" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="W36" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="X36" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y36" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z36" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA36" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB36" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC36" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD36" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="18:69" x14ac:dyDescent="0.2">
+      <c r="R37" s="2">
+        <v>6</v>
+      </c>
+      <c r="T37" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="U37" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="V37" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="W37" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="X37" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y37" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z37" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA37" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB37" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC37" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD37" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="18:69" x14ac:dyDescent="0.2">
+      <c r="R38" s="2">
+        <v>9</v>
+      </c>
+      <c r="T38" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="U38" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="V38" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="W38" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="X38" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y38" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z38" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA38" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB38" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC38" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD38" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="18:69" x14ac:dyDescent="0.2">
+      <c r="R39" s="2">
+        <v>5</v>
+      </c>
+      <c r="U39" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="V39" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="W39" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="X39" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y39" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z39" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA39" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB39" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC39" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="18:69" x14ac:dyDescent="0.2">
+      <c r="AH42" s="2">
+        <v>13</v>
+      </c>
+      <c r="AI42" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43" spans="18:69" x14ac:dyDescent="0.2">
+      <c r="AH43" s="2">
+        <v>11</v>
+      </c>
+      <c r="AI43" s="2" t="s">
+        <v>21</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>